<commit_message>
fixed attitude data output
</commit_message>
<xml_diff>
--- a/gt_data_transformation/181224_setup.xlsx
+++ b/gt_data_transformation/181224_setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xwb18136\OneDrive - University of Strathclyde\Documents\GitHub\proxima-lab\gt_data_transformation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29A00BB-2683-4A30-B79E-7D043DAEF65F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801A9F1B-AF84-40A0-9423-1515E7E7AAF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -395,7 +395,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,6 +528,9 @@
       <c r="C6">
         <v>0</v>
       </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
       <c r="E6">
         <v>0</v>
       </c>

</xml_diff>